<commit_message>
Completed final project and documentation for Incident Response & Digital Forensics. Added README, finalized Solution document, and uploaded related lab and reference materials. Also updated Agile course folder.
Add final IR/Forensics project, lab documentation, and Agile course update

- Finalized and uploaded Incident Response & Digital Forensics project (NIST-based)
- Added lab screenshots and notes for OS/Security coursework
- Completed Agile Process, Project & Program Controls class; updated README
- Organized all files for GitHub portfolio structure
</commit_message>
<xml_diff>
--- a/2025_Course_Tracker_Portfolio_NM.xlsx
+++ b/2025_Course_Tracker_Portfolio_NM.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\Portfolio work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\GitHub\cybersecurity-portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F074A162-4BDC-4CE7-B125-F8E8E505D67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5A039E-63E5-483A-AFBB-4ECC6570D714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
   </bookViews>
   <sheets>
     <sheet name="Training_Progress_Tracker" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="168">
   <si>
     <t>Course</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Sound the Alarm - Detection &amp; Response</t>
   </si>
   <si>
-    <t>Tools for the Trade - Linux &amp; SQL</t>
-  </si>
-  <si>
     <t>Accelerate Your Job Search with AI</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
   </si>
   <si>
     <t>Python Basics for Data Science</t>
-  </si>
-  <si>
-    <t>IN PROGRESS</t>
   </si>
   <si>
     <t>CS50 - Introduction to Cybersecurity</t>
@@ -417,29 +411,6 @@
     <t>Use screenshots or sanitized logs if needed</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Build repo: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>/incident-response</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> with templates</t>
-    </r>
-  </si>
-  <si>
     <t>Even just logs + markdown write-up</t>
   </si>
   <si>
@@ -558,9 +529,6 @@
     <t>High Priority: Add recon/exploit scripts or labs (if legal/public)</t>
   </si>
   <si>
-    <t>High Priority: Create IR playbook or forensics workflow</t>
-  </si>
-  <si>
     <t>High Priority: Add firewall configs or packet analysis</t>
   </si>
   <si>
@@ -580,6 +548,42 @@
   </si>
   <si>
     <t>Medium Priority: Add shell scripts or terminal output with comments</t>
+  </si>
+  <si>
+    <t>IN Progress</t>
+  </si>
+  <si>
+    <t>Sprint Planning for Faster Agile Team Delivery</t>
+  </si>
+  <si>
+    <t>EdX - UMD</t>
+  </si>
+  <si>
+    <t>Agile Leadership Principles &amp; Practices</t>
+  </si>
+  <si>
+    <t>Agile Innovation &amp; Problem Solving</t>
+  </si>
+  <si>
+    <t>EdX - UD</t>
+  </si>
+  <si>
+    <t>Tools for the Trade - Linux &amp; SQL+A29A40A1:A42</t>
+  </si>
+  <si>
+    <t>Agile Mindset</t>
+  </si>
+  <si>
+    <t>Agile Leadership</t>
+  </si>
+  <si>
+    <t>Sprint Planning</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -734,7 +738,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -935,6 +939,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1153,7 +1163,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1166,7 +1176,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1184,6 +1193,8 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1539,11 +1550,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45A587F-D2B6-447F-B3AB-8D0BEB05BA92}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M3" sqref="M3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1557,63 +1568,63 @@
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.26953125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="14.08984375" style="15" customWidth="1"/>
+    <col min="10" max="10" width="8.26953125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="14.08984375" style="14" customWidth="1"/>
     <col min="13" max="13" width="58.90625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="40.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42.54296875" style="11" customWidth="1"/>
+    <col min="15" max="15" width="42.54296875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="15" customFormat="1" ht="29.5" thickBot="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:15" s="14" customFormat="1" ht="29.5" thickBot="1">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>115</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="29" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
@@ -1623,456 +1634,443 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" s="6">
         <v>45867</v>
       </c>
       <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" t="s">
         <v>65</v>
       </c>
-      <c r="H2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>145</v>
+      <c r="J2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="N2" t="s">
-        <v>118</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>130</v>
+        <v>116</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="29" customHeight="1">
       <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="8">
         <v>45855</v>
       </c>
       <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" t="s">
         <v>68</v>
       </c>
-      <c r="H3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>52</v>
+      <c r="J3" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" t="s">
-        <v>139</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="29.5" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>37</v>
+        <v>160</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>36</v>
+        <v>161</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>54</v>
+        <v>167</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I4" t="s">
         <v>68</v>
       </c>
-      <c r="H4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>52</v>
-      </c>
       <c r="M4" s="2"/>
-      <c r="N4" s="10"/>
-    </row>
-    <row r="5" spans="1:15" ht="56" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="29.5" customHeight="1">
+      <c r="A5" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>164</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" ht="28" customHeight="1">
+    </row>
+    <row r="6" spans="1:15" ht="29.5" customHeight="1">
       <c r="A6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="8">
-        <v>45866</v>
+        <v>45872</v>
       </c>
       <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
         <v>68</v>
       </c>
-      <c r="H6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" ht="56" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" t="s">
         <v>70</v>
       </c>
-      <c r="J6" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" t="s">
-        <v>131</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="42.5" customHeight="1">
-      <c r="A7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="8">
-        <v>45817</v>
-      </c>
-      <c r="G7" t="s">
-        <v>76</v>
-      </c>
       <c r="H7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>147</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="11" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="8" spans="1:15" ht="28" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" s="8">
-        <v>45867</v>
+        <v>45866</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="O8" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="42.5" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="8">
+        <v>45817</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="28" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="8">
+        <v>45867</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="8">
         <v>45785</v>
       </c>
-      <c r="G9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="4">
+        <v>45764</v>
+      </c>
+      <c r="G12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" t="s">
         <v>81</v>
       </c>
-      <c r="I9" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="I12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="4">
-        <v>45764</v>
-      </c>
-      <c r="G10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I10" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" t="s">
-        <v>85</v>
-      </c>
-      <c r="I11" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" ht="29">
-      <c r="A12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="8">
-        <v>45808</v>
-      </c>
-      <c r="G12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>127</v>
+      <c r="K12" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>76</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" ht="29">
       <c r="A14" s="7" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="8">
-        <v>45748</v>
+        <v>45808</v>
       </c>
       <c r="G14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" t="s">
         <v>76</v>
       </c>
-      <c r="H14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>52</v>
+      <c r="J14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2080,665 +2078,666 @@
         <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I15" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>52</v>
+        <v>68</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="8">
-        <v>45755</v>
+        <v>45748</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I16" t="s">
-        <v>91</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="N16" t="s">
-        <v>133</v>
-      </c>
-      <c r="O16" s="11" t="s">
-        <v>134</v>
+        <v>76</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="8">
-        <v>45799</v>
-      </c>
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="H17" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="43.5">
+        <v>88</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F18" s="8">
-        <v>45764</v>
+        <v>45755</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="H18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M18" s="17" t="s">
-        <v>149</v>
+        <v>89</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="N18" t="s">
-        <v>137</v>
-      </c>
-      <c r="O18" s="11" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="E19" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" s="8">
-        <v>45791</v>
+        <v>45799</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I19" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="O19" s="11" t="s">
-        <v>126</v>
+        <v>76</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="43.5">
       <c r="A20" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="E20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" s="8">
-        <v>45779</v>
+        <v>45764</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>52</v>
+        <v>76</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="N20" t="s">
-        <v>143</v>
-      </c>
-      <c r="O20" s="11" t="s">
-        <v>144</v>
+        <v>134</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="A21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="8">
+        <v>45791</v>
+      </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="H21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I21" t="s">
-        <v>97</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+        <v>76</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="43.5">
       <c r="A22" s="7" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" s="8">
-        <v>45797</v>
+        <v>45779</v>
       </c>
       <c r="G22" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" t="s">
         <v>76</v>
       </c>
-      <c r="H22" t="s">
-        <v>98</v>
-      </c>
-      <c r="I22" t="s">
-        <v>82</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>52</v>
+      <c r="J22" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="N22" t="s">
+        <v>140</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H23" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I23" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K23" s="15" t="s">
-        <v>52</v>
+        <v>95</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="8">
+        <v>45797</v>
+      </c>
       <c r="G24" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="H24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I24" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K24" s="15" t="s">
-        <v>52</v>
+        <v>80</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K25" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M25" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="O25" s="11" t="s">
-        <v>125</v>
+        <v>65</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="8">
-        <v>45790</v>
-      </c>
+      <c r="A26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="G26" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="H26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I26" t="s">
-        <v>82</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K26" s="15" t="s">
-        <v>52</v>
+        <v>65</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="7" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27" s="8">
-        <v>45819</v>
+        <v>45872</v>
       </c>
       <c r="G27" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H27" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I27" t="s">
-        <v>82</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K27" s="15" t="s">
-        <v>52</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M27" s="15"/>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F28" s="8">
-        <v>45744</v>
+        <v>45790</v>
       </c>
       <c r="G28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I28" t="s">
-        <v>82</v>
-      </c>
-      <c r="J28" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>52</v>
+        <v>80</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" s="8">
-        <v>45780</v>
+        <v>45819</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H29" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M29" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="O29" s="11" t="s">
-        <v>124</v>
+        <v>80</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="D30" s="7"/>
       <c r="E30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" s="8">
-        <v>45756</v>
+        <v>45744</v>
       </c>
       <c r="G30" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" t="s">
+        <v>102</v>
+      </c>
+      <c r="I30" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="8">
+        <v>45780</v>
+      </c>
+      <c r="G31" t="s">
+        <v>82</v>
+      </c>
+      <c r="H31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" t="s">
         <v>76</v>
       </c>
-      <c r="H30" t="s">
-        <v>105</v>
-      </c>
-      <c r="I30" t="s">
-        <v>78</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M30" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="O30" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="29">
-      <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" t="s">
-        <v>84</v>
-      </c>
-      <c r="H31" t="s">
-        <v>106</v>
-      </c>
-      <c r="I31" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K31" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M31" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="O31" s="11" t="s">
+      <c r="J31" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M31" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="O31" s="10" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="E32" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F32" s="8">
-        <v>45799</v>
+        <v>45756</v>
       </c>
       <c r="G32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" t="s">
+        <v>103</v>
+      </c>
+      <c r="I32" t="s">
         <v>76</v>
       </c>
-      <c r="H32" t="s">
-        <v>107</v>
-      </c>
-      <c r="I32" t="s">
-        <v>78</v>
-      </c>
-      <c r="J32" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K32" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="J32" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M32" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="O32" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="29">
+      <c r="A33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
       <c r="G33" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="H33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I33" t="s">
-        <v>67</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K33" s="15" t="s">
-        <v>52</v>
+        <v>76</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M33" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>7</v>
@@ -2748,189 +2747,180 @@
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F34" s="8">
-        <v>45868</v>
+        <v>45799</v>
       </c>
       <c r="G34" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" t="s">
+        <v>105</v>
+      </c>
+      <c r="I34" t="s">
         <v>76</v>
       </c>
-      <c r="H34" t="s">
-        <v>109</v>
-      </c>
-      <c r="I34" t="s">
-        <v>110</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K34" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="N34" t="s">
-        <v>135</v>
-      </c>
-      <c r="O34" s="11" t="s">
-        <v>136</v>
+      <c r="J34" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="8">
-        <v>45840</v>
-      </c>
+      <c r="A35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="G35" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="H35" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I35" t="s">
-        <v>78</v>
-      </c>
-      <c r="J35" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K35" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M35" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="O35" s="11" t="s">
-        <v>121</v>
+        <v>65</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="7" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="7"/>
+      <c r="E36" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="8">
+        <v>45868</v>
+      </c>
+      <c r="G36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H36" t="s">
+        <v>107</v>
+      </c>
+      <c r="I36" t="s">
+        <v>108</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="N36" t="s">
+        <v>132</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="8">
-        <v>45809</v>
-      </c>
-      <c r="G36" t="s">
-        <v>92</v>
-      </c>
-      <c r="H36" t="s">
-        <v>94</v>
-      </c>
-      <c r="I36" t="s">
-        <v>78</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K36" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M36" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="O36" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="29">
-      <c r="A37" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="B37" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="D37" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="E37" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F37" s="8">
-        <v>45855</v>
+        <v>45840</v>
       </c>
       <c r="G37" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I37" t="s">
-        <v>78</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K37" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M37" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="N37" t="s">
-        <v>141</v>
-      </c>
-      <c r="O37" s="11" t="s">
-        <v>142</v>
+        <v>76</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="O37" s="10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="A38" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="8">
+        <v>45809</v>
+      </c>
       <c r="G38" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="H38" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="I38" t="s">
-        <v>67</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K38" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15">
+        <v>76</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M38" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="O38" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="29">
       <c r="A39" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>7</v>
@@ -2940,36 +2930,131 @@
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F39" s="8">
+        <v>45855</v>
+      </c>
+      <c r="G39" t="s">
+        <v>82</v>
+      </c>
+      <c r="H39" t="s">
+        <v>110</v>
+      </c>
+      <c r="I39" t="s">
+        <v>76</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M39" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="N39" t="s">
+        <v>138</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="18"/>
+      <c r="G40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" t="s">
+        <v>165</v>
+      </c>
+      <c r="I40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M40" s="15"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H41" t="s">
+        <v>111</v>
+      </c>
+      <c r="I41" t="s">
+        <v>65</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" s="8">
         <v>45820</v>
       </c>
-      <c r="G39" t="s">
-        <v>92</v>
-      </c>
-      <c r="H39" t="s">
-        <v>114</v>
-      </c>
-      <c r="I39" t="s">
-        <v>78</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K39" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="O39" s="11" t="s">
-        <v>119</v>
+      <c r="G42" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" t="s">
+        <v>112</v>
+      </c>
+      <c r="I42" t="s">
+        <v>76</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K42" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M42" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="O42" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F39">
-    <sortCondition ref="A1:A39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F42">
+    <sortCondition ref="A1:A42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add finalized labs, technical assignments, and updated READMEs
This push includes:

✅ Finalized RSA Encryption, AES Encryption, and DES Cryptanalysis lab documents (PDF)

✅ New and updated README.md files across multiple modules

✅ Uploaded threat reports, NMap GUI, CLI exercises, and other technical assignment outputs

✅ Added badge and certificate assets to Badges and Certificates/

✅ Updated 2025 course tracking Excel file

Organized and documented for GitHub portfolio visibility and reviewer clarity.
</commit_message>
<xml_diff>
--- a/2025_Course_Tracker_Portfolio_NM.xlsx
+++ b/2025_Course_Tracker_Portfolio_NM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\GitHub\cybersecurity-portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5A039E-63E5-483A-AFBB-4ECC6570D714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB206C3-0F74-4985-A1A9-4382E075E276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
   </bookViews>
   <sheets>
     <sheet name="Training_Progress_Tracker" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="168">
   <si>
     <t>Course</t>
   </si>
@@ -1554,7 +1554,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J8" sqref="J8"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1705,18 +1705,22 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="29.5" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="8">
+        <v>45875</v>
+      </c>
       <c r="G4" t="s">
         <v>66</v>
       </c>
@@ -1729,18 +1733,18 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="29.5" customHeight="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
       <c r="G5" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Add course tracker, certificates, case studies, and final project deliverables
Added updated 2025_Course_Tracker_Portfolio_NM.xlsx for coursework tracking

Uploaded certificates: Agile Leadership, Phishing Threats, and Penetration Testing/Threat Hunting/Cryptography

Added case study PDFs: Deep Fake, Home Depot, and Pegasus Airlines

Uploaded final project deliverables:

Part 1: Penetration Testing, Threat Hunting, and Cryptography

Part 2: Secure Information Using Symmetric Encryption
</commit_message>
<xml_diff>
--- a/2025_Course_Tracker_Portfolio_NM.xlsx
+++ b/2025_Course_Tracker_Portfolio_NM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\GitHub\cybersecurity-portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB206C3-0F74-4985-A1A9-4382E075E276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFE1161-55DF-4AB9-8891-B0CB93CC3FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
+    <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
   </bookViews>
   <sheets>
     <sheet name="Training_Progress_Tracker" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="165">
   <si>
     <t>Course</t>
   </si>
@@ -380,9 +380,6 @@
   </si>
   <si>
     <t>Combine with the automation repo if needed</t>
-  </si>
-  <si>
-    <t>Create dedicated repo if substantial hands-on work</t>
   </si>
   <si>
     <r>
@@ -535,9 +532,6 @@
     <t>Medium Priority: Bash scripts, config examples</t>
   </si>
   <si>
-    <t>High Priority: Push any testing frameworks or encryption labs</t>
-  </si>
-  <si>
     <t>High Priority: Push notebooks or .py files</t>
   </si>
   <si>
@@ -550,9 +544,6 @@
     <t>Medium Priority: Add shell scripts or terminal output with comments</t>
   </si>
   <si>
-    <t>IN Progress</t>
-  </si>
-  <si>
     <t>Sprint Planning for Faster Agile Team Delivery</t>
   </si>
   <si>
@@ -583,7 +574,7 @@
     <t>COMPLETED</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>IN PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -738,7 +729,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,12 +930,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1163,7 +1148,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1193,8 +1178,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1552,9 +1536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45A587F-D2B6-447F-B3AB-8D0BEB05BA92}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="A17" sqref="A17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1655,13 +1639,13 @@
         <v>51</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N2" t="s">
         <v>116</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="29" customHeight="1">
@@ -1698,18 +1682,18 @@
       </c>
       <c r="M3" s="2"/>
       <c r="N3" t="s">
+        <v>135</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="29.5" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -1725,7 +1709,7 @@
         <v>66</v>
       </c>
       <c r="H4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I4" t="s">
         <v>68</v>
@@ -1733,26 +1717,36 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="29.5" customHeight="1">
-      <c r="A5" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="A5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="8">
+        <v>45892</v>
+      </c>
       <c r="G5" t="s">
         <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I5" t="s">
         <v>68</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="M5" s="2"/>
     </row>
@@ -1764,7 +1758,7 @@
         <v>35</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
@@ -1855,10 +1849,10 @@
       </c>
       <c r="M8" s="2"/>
       <c r="N8" t="s">
+        <v>127</v>
+      </c>
+      <c r="O8" s="10" t="s">
         <v>128</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="42.5" customHeight="1">
@@ -1894,11 +1888,11 @@
         <v>51</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="28" customHeight="1">
@@ -1934,11 +1928,11 @@
         <v>51</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -2071,10 +2065,10 @@
         <v>51</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2142,18 +2136,18 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="C17" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
       <c r="G17" t="s">
         <v>70</v>
       </c>
@@ -2205,10 +2199,10 @@
         <v>51</v>
       </c>
       <c r="N18" t="s">
+        <v>129</v>
+      </c>
+      <c r="O18" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="O18" s="10" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -2281,13 +2275,13 @@
         <v>51</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N20" t="s">
+        <v>133</v>
+      </c>
+      <c r="O20" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="O20" s="10" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -2323,10 +2317,10 @@
         <v>51</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="43.5">
@@ -2362,13 +2356,13 @@
         <v>51</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N22" t="s">
+        <v>139</v>
+      </c>
+      <c r="O22" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="O22" s="10" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -2657,10 +2651,10 @@
         <v>51</v>
       </c>
       <c r="M31" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2698,25 +2692,27 @@
         <v>51</v>
       </c>
       <c r="M32" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="29">
-      <c r="A33" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
+      <c r="C33" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8">
+        <v>45894</v>
+      </c>
       <c r="G33" t="s">
         <v>82</v>
       </c>
@@ -2732,12 +2728,7 @@
       <c r="K33" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="M33" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="O33" s="10" t="s">
-        <v>120</v>
-      </c>
+      <c r="M33" s="15"/>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="7" t="s">
@@ -2834,10 +2825,10 @@
         <v>51</v>
       </c>
       <c r="N36" t="s">
+        <v>131</v>
+      </c>
+      <c r="O36" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="O36" s="10" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -2875,7 +2866,7 @@
         <v>51</v>
       </c>
       <c r="M37" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O37" s="10" t="s">
         <v>119</v>
@@ -2916,7 +2907,7 @@
         <v>51</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O38" s="10" t="s">
         <v>118</v>
@@ -2955,33 +2946,33 @@
         <v>51</v>
       </c>
       <c r="M39" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N39" t="s">
+        <v>137</v>
+      </c>
+      <c r="O39" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="O39" s="10" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="40" spans="1:15">
-      <c r="A40" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="18"/>
+      <c r="A40" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="17"/>
       <c r="G40" t="s">
         <v>66</v>
       </c>
       <c r="H40" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I40" t="s">
         <v>68</v>
@@ -3019,7 +3010,7 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>7</v>
@@ -3050,7 +3041,7 @@
         <v>51</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O42" s="10" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
Added course overviews and lab documentation for Digital Forensics Essentials, Ethical Hacking Fundamentals, Network Defense Essentials, and Tools of the Trade: Linux and SQL. Updated repository with structured lab files and course summaries.
This update includes multiple finalized course overviews and lab writeups across four main technical areas. Each course folder now contains organized PDF files for individual labs and a one-page course overview. The additions cover forensic techniques, ethical hacking modules, network defense topics, and Linux/SQL command activities. The repository structure has been aligned for consistency and portfolio readiness, ensuring that all technical assignments and supporting documents are captured for reference and review.
</commit_message>
<xml_diff>
--- a/2025_Course_Tracker_Portfolio_NM.xlsx
+++ b/2025_Course_Tracker_Portfolio_NM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\GitHub\Cybersecurity Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA126BB9-90E7-4355-91A4-6C9062A410CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE50590-E799-44CC-8D92-92E77F3BE0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Training_Progress_Tracker" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="201">
   <si>
     <t>Course</t>
   </si>
@@ -475,28 +476,10 @@
     <t>Paralegal Studies</t>
   </si>
   <si>
-    <t>upload lab reports or artifacts from forensic labs</t>
-  </si>
-  <si>
-    <t>highlight practical forensic exercises (disk imaging, evidence handling, chain of custody</t>
-  </si>
-  <si>
     <t>Completed technical forensics course. Labs included; upload lab artifacts to GitHub with README summary</t>
   </si>
   <si>
-    <t>upload lab work (scanning, vulnerability testing, exploitation basics</t>
-  </si>
-  <si>
-    <t>showcase ethical hacking workflow and lab outputs</t>
-  </si>
-  <si>
     <t>Completed technical ethical hacking course. Labs included; upload lab reports to GitHub with README summary</t>
-  </si>
-  <si>
-    <t>upload lab results (firewall configs, IDS/IPS exercises, defense setups</t>
-  </si>
-  <si>
-    <t>emphasize defensive configurations and network monitoring labs</t>
   </si>
   <si>
     <t>Completed technical network defense course. Labs included; upload lab artifacts to GitHub with README summary</t>
@@ -614,12 +597,6 @@
   </si>
   <si>
     <t>Covered IR lifecycle (NIST), Wireshark/tcpdump labs, IDS/IPS (Suricata), SIEM queries (Splunk, Chronicle). Final project: incident journal with 5 W’s, tools, and response documentation.</t>
-  </si>
-  <si>
-    <t>Linux &amp; SQL Final Lab (Linux commands, file permissions, SQL queries in terminal)</t>
-  </si>
-  <si>
-    <t>Already in GitHub — add README if missing</t>
   </si>
   <si>
     <t>Covered Linux basics (shell, file system, permissions) and SQL querying (CRUD ops, joins, filters). Final project: run Linux CLI tasks and SQL queries, submit outputs.</t>
@@ -676,6 +653,12 @@
   </si>
   <si>
     <t>Upload, done/Readme, done/ overview done</t>
+  </si>
+  <si>
+    <t>Overview Done</t>
+  </si>
+  <si>
+    <t>Overview done</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1278,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1309,17 +1292,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1454,6 +1430,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1813,7 +1795,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -1830,9 +1812,9 @@
     <col min="10" max="10" width="10.3046875" style="4" customWidth="1"/>
     <col min="11" max="11" width="14.07421875" style="4" customWidth="1"/>
     <col min="12" max="12" width="8.69140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="58.921875" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.4609375" style="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42.53515625" style="28" customWidth="1"/>
+    <col min="13" max="13" width="58.921875" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.4609375" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42.53515625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="65.599999999999994" customHeight="1" thickBot="1">
@@ -1854,28 +1836,28 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="27" t="s">
         <v>99</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -1883,825 +1865,825 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="29.05" customHeight="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="17">
+      <c r="E2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="14">
         <v>45867</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="26" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="49" customFormat="1" ht="102">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:15" s="46" customFormat="1" ht="102">
+      <c r="A3" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="46">
+      <c r="E3" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="43">
         <v>45855</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="45"/>
-      <c r="M3" s="48" t="s">
+      <c r="J3" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="N3" s="54" t="s">
-        <v>206</v>
-      </c>
-      <c r="O3" s="47" t="s">
-        <v>205</v>
+      <c r="N3" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="O3" s="44" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="29.5" customHeight="1">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="46">
+      <c r="D4" s="42"/>
+      <c r="E4" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="43">
         <v>45875</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" s="45"/>
-      <c r="M4" s="47" t="s">
+      <c r="K4" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N4" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="O4" s="47" t="s">
+      <c r="N4" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="O4" s="44" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="49" customFormat="1" ht="29.5" customHeight="1">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:15" s="46" customFormat="1" ht="29.5" customHeight="1">
+      <c r="A5" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="46">
+      <c r="D5" s="42"/>
+      <c r="E5" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="43">
         <v>45892</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="45"/>
-      <c r="M5" s="48" t="s">
+      <c r="K5" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="42"/>
+      <c r="M5" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="O5" s="47" t="s">
+      <c r="N5" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="O5" s="44" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="49" customFormat="1" ht="29.5" customHeight="1">
-      <c r="A6" s="44" t="s">
+    <row r="6" spans="1:15" s="46" customFormat="1" ht="29.5" customHeight="1">
+      <c r="A6" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="46">
+      <c r="D6" s="42"/>
+      <c r="E6" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="43">
         <v>45872</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="45" t="s">
+      <c r="H6" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="45" t="s">
+      <c r="I6" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="45" t="s">
+      <c r="J6" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="45"/>
-      <c r="M6" s="47" t="s">
+      <c r="K6" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="42"/>
+      <c r="M6" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N6" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="O6" s="47" t="s">
+      <c r="N6" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="O6" s="44" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="49" customFormat="1" ht="28" customHeight="1">
-      <c r="A7" s="44" t="s">
+    <row r="7" spans="1:15" s="46" customFormat="1" ht="28" customHeight="1">
+      <c r="A7" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="46">
+      <c r="D7" s="42"/>
+      <c r="E7" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="43">
         <v>45866</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="45" t="s">
+      <c r="I7" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="45"/>
-      <c r="M7" s="47" t="s">
+      <c r="K7" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="42"/>
+      <c r="M7" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N7" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="O7" s="47" t="s">
+      <c r="N7" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="O7" s="44" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="55" customFormat="1" ht="87.45">
-      <c r="A8" s="44" t="s">
+    <row r="8" spans="1:15" s="52" customFormat="1" ht="87.45">
+      <c r="A8" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="46">
+      <c r="D8" s="42"/>
+      <c r="E8" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="43">
         <v>45817</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="45"/>
-      <c r="M8" s="47" t="s">
+      <c r="J8" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="42"/>
+      <c r="M8" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N8" s="54" t="s">
-        <v>206</v>
-      </c>
-      <c r="O8" s="47" t="s">
+      <c r="N8" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="O8" s="44" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="72.900000000000006">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="46">
+      <c r="D9" s="42"/>
+      <c r="E9" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="43">
         <v>45867</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="45" t="s">
+      <c r="I9" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="45"/>
-      <c r="M9" s="47" t="s">
+      <c r="J9" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="42"/>
+      <c r="M9" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N9" s="47" t="s">
-        <v>206</v>
-      </c>
-      <c r="O9" s="47" t="s">
+      <c r="N9" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="O9" s="44" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="49" customFormat="1" ht="43.75">
-      <c r="A10" s="44" t="s">
+    <row r="10" spans="1:15" s="46" customFormat="1" ht="43.75">
+      <c r="A10" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="46">
+      <c r="D10" s="42"/>
+      <c r="E10" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="43">
         <v>45785</v>
       </c>
-      <c r="G10" s="45" t="s">
+      <c r="G10" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="H10" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="45" t="s">
+      <c r="I10" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="45" t="s">
+      <c r="J10" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45" t="s">
+      <c r="K10" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="N10" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="O10" s="47" t="s">
+      <c r="N10" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="O10" s="44" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
     </row>
     <row r="12" spans="1:15" ht="30.45" customHeight="1">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="46">
+      <c r="D12" s="42"/>
+      <c r="E12" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="43">
         <v>45808</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="45" t="s">
+      <c r="H12" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="45" t="s">
+      <c r="I12" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45" t="s">
+      <c r="J12" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="N12" s="54" t="s">
-        <v>206</v>
-      </c>
-      <c r="O12" s="47"/>
+      <c r="N12" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="O12" s="44"/>
     </row>
     <row r="13" spans="1:15" ht="87.45">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="24">
+      <c r="D13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="21">
         <v>45748</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="25" t="s">
+      <c r="J13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="N13" s="25" t="s">
+      <c r="N13" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="O13" s="25" t="s">
+      <c r="O13" s="22" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="29.15">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="24">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="21">
         <v>45900</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="J14" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="25" t="s">
+      <c r="J14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="11"/>
+      <c r="M14" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="N14" s="25" t="s">
+      <c r="N14" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="O14" s="25" t="s">
+      <c r="O14" s="22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="49" customFormat="1" ht="43.75">
-      <c r="A15" s="44" t="s">
+    <row r="15" spans="1:15" s="46" customFormat="1" ht="43.75">
+      <c r="A15" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="46">
+      <c r="D15" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="43">
         <v>45755</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G15" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H15" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="45" t="s">
+      <c r="I15" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="45" t="s">
+      <c r="J15" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L15" s="45"/>
-      <c r="M15" s="47" t="s">
+      <c r="K15" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="42"/>
+      <c r="M15" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N15" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="O15" s="47" t="s">
+      <c r="N15" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="O15" s="44" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="49" customFormat="1" ht="43.75">
-      <c r="A16" s="44" t="s">
+    <row r="16" spans="1:15" s="46" customFormat="1" ht="43.75">
+      <c r="A16" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="46">
+      <c r="D16" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="43">
         <v>45799</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="H16" s="45" t="s">
+      <c r="H16" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="I16" s="45" t="s">
+      <c r="I16" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="J16" s="45" t="s">
+      <c r="J16" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L16" s="45"/>
-      <c r="M16" s="47" t="s">
+      <c r="K16" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="42"/>
+      <c r="M16" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N16" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O16" s="47" t="s">
+      <c r="N16" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O16" s="44" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="49" customFormat="1" ht="29.15">
-      <c r="A17" s="44" t="s">
+    <row r="17" spans="1:15" s="46" customFormat="1" ht="29.15">
+      <c r="A17" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="46">
+      <c r="D17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="43">
         <v>45764</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="H17" s="45" t="s">
+      <c r="H17" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="45" t="s">
+      <c r="I17" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="45" t="s">
+      <c r="J17" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K17" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L17" s="45"/>
-      <c r="M17" s="47" t="s">
+      <c r="K17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="42"/>
+      <c r="M17" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N17" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O17" s="47" t="s">
+      <c r="N17" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O17" s="44" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="43.75">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="18">
+      <c r="D18" s="42"/>
+      <c r="E18" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="43">
         <v>45791</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="5" t="s">
+      <c r="J18" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="N18" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="O18" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="N18" s="12" t="s">
+    </row>
+    <row r="19" spans="1:15" ht="43.75">
+      <c r="A19" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="43">
+        <v>45779</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="N19" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="O19" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="O18" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="43.75">
-      <c r="A19" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="18">
-        <v>45779</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" s="11"/>
-      <c r="M19" s="5" t="s">
+    </row>
+    <row r="20" spans="1:15" s="46" customFormat="1" ht="87.45">
+      <c r="A20" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="43">
+        <v>45902</v>
+      </c>
+      <c r="G20" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="42"/>
+      <c r="M20" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N20" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O20" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="N19" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="O19" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="49" customFormat="1" ht="87.45">
-      <c r="A20" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="46">
-        <v>45902</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="J20" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="K20" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20" s="45"/>
-      <c r="M20" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="N20" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O20" s="50" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="37"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="34"/>
       <c r="G21" s="4" t="s">
         <v>148</v>
       </c>
@@ -2712,1021 +2694,1021 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="49" customFormat="1" ht="29.15">
-      <c r="A22" s="44" t="s">
+    <row r="22" spans="1:15" s="46" customFormat="1" ht="29.15">
+      <c r="A22" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="46">
+      <c r="D22" s="42"/>
+      <c r="E22" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="43">
         <v>45797</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="45" t="s">
+      <c r="H22" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="I22" s="45" t="s">
+      <c r="I22" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="45" t="s">
+      <c r="J22" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L22" s="45"/>
-      <c r="M22" s="47" t="s">
+      <c r="K22" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" s="42"/>
+      <c r="M22" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N22" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O22" s="50" t="s">
+      <c r="N22" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O22" s="47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="46" customFormat="1" ht="58.3">
+      <c r="A23" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="48">
+        <v>45909</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K23" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" s="42"/>
+      <c r="M23" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N23" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O23" s="47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="46" customFormat="1" ht="43.75">
+      <c r="A24" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="43">
+        <v>45907</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L24" s="42"/>
+      <c r="M24" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N24" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O24" s="47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="46" customFormat="1" ht="72.900000000000006">
+      <c r="A25" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="43">
+        <v>45904</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K25" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L25" s="42"/>
+      <c r="M25" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N25" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O25" s="47" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="46" customFormat="1" ht="72.900000000000006">
+      <c r="A26" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="43">
+        <v>45905</v>
+      </c>
+      <c r="G26" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="H26" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="I26" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="42"/>
+      <c r="M26" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N26" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O26" s="47" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="43.75">
+      <c r="A27" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="35">
+        <v>45872</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" s="11"/>
+      <c r="M27" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="O27" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="58.3">
+      <c r="A28" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="15">
+        <v>45790</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="8"/>
+      <c r="M28" s="18" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" s="49" customFormat="1" ht="58.3">
-      <c r="A23" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="45" t="s">
+      <c r="N28" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="O28" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="46" customFormat="1" ht="58.3">
+      <c r="A29" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="43">
+        <v>45819</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="I29" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="J29" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K29" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29" s="42"/>
+      <c r="M29" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N29" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O29" s="47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="43.75">
+      <c r="A30" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="21">
+        <v>45902</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L30" s="11"/>
+      <c r="M30" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="N30" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="46" customFormat="1" ht="72.900000000000006">
+      <c r="A31" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="43">
+        <v>45744</v>
+      </c>
+      <c r="G31" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H31" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="I31" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K31" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31" s="42"/>
+      <c r="M31" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N31" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O31" s="47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="43.75">
+      <c r="A32" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="43">
+        <v>45780</v>
+      </c>
+      <c r="G32" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="H32" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="I32" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="J32" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="N32" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="O32" s="47" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="46" customFormat="1" ht="43.75">
+      <c r="A33" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="43">
+        <v>45903</v>
+      </c>
+      <c r="G33" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="I33" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="J33" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K33" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L33" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="M33" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N33" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="O33" s="44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="52.3" customHeight="1">
+      <c r="A34" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="15">
+        <v>45756</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="O34" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="102" customHeight="1">
+      <c r="A35" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C35" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="21">
+        <v>45894</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L35" s="11"/>
+      <c r="M35" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="46" customFormat="1" ht="58.3">
+      <c r="A36" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="51">
-        <v>45909</v>
-      </c>
-      <c r="G23" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="H23" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="I23" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" s="45" t="s">
+      <c r="D36" s="50"/>
+      <c r="E36" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="43">
+        <v>45799</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I36" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="J36" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="K23" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L23" s="45"/>
-      <c r="M23" s="47" t="s">
+      <c r="K36" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L36" s="42"/>
+      <c r="M36" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N23" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O23" s="50" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" s="49" customFormat="1" ht="43.75">
-      <c r="A24" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="45" t="s">
+      <c r="N36" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="O36" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="58.3">
+      <c r="A37" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="46">
-        <v>45907</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="H24" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="I24" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="J24" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="K24" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L24" s="45"/>
-      <c r="M24" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="N24" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O24" s="50" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" s="49" customFormat="1" ht="72.900000000000006">
-      <c r="A25" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="45" t="s">
+      <c r="D37" s="8"/>
+      <c r="E37" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" s="36">
+        <v>45868</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L37" s="8"/>
+      <c r="M37" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="N37" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="O37" s="18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="58.3">
+      <c r="A38" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="46">
-        <v>45904</v>
-      </c>
-      <c r="G25" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="I25" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="K25" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L25" s="45"/>
-      <c r="M25" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="N25" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O25" s="50" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="49" customFormat="1" ht="72.900000000000006">
-      <c r="A26" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="45" t="s">
+      <c r="D38" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="15">
+        <v>45840</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L38" s="8"/>
+      <c r="M38" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="N38" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="O38" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="72.900000000000006">
+      <c r="A39" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="46">
-        <v>45905</v>
-      </c>
-      <c r="G26" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="H26" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="I26" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="K26" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="45"/>
-      <c r="M26" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="N26" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O26" s="50" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="43.75">
-      <c r="A27" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="38">
-        <v>45872</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="I27" s="14" t="s">
+      <c r="D39" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="36">
+        <v>45809</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J27" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" s="14"/>
-      <c r="M27" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="N27" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="O27" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="58.3">
-      <c r="A28" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="18">
-        <v>45790</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="N28" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="O28" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" s="49" customFormat="1" ht="58.3">
-      <c r="A29" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="46">
-        <v>45819</v>
-      </c>
-      <c r="G29" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="I29" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="J29" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="K29" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L29" s="45"/>
-      <c r="M29" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="N29" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O29" s="50" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="43.75">
-      <c r="A30" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="24">
-        <v>45902</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L30" s="14"/>
-      <c r="M30" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="N30" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="O30" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="49" customFormat="1" ht="72.900000000000006">
-      <c r="A31" s="44" t="s">
-        <v>204</v>
-      </c>
-      <c r="B31" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="46">
-        <v>45744</v>
-      </c>
-      <c r="G31" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="H31" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="I31" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="J31" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="K31" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L31" s="45"/>
-      <c r="M31" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="N31" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O31" s="50" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="43.75">
-      <c r="A32" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="18">
-        <v>45780</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L32" s="11"/>
-      <c r="M32" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="O32" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="49" customFormat="1" ht="43.75">
-      <c r="A33" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="46">
-        <v>45903</v>
-      </c>
-      <c r="G33" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="H33" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="I33" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="J33" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="K33" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L33" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="M33" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="N33" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="O33" s="47" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="52.3" customHeight="1">
-      <c r="A34" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="18">
-        <v>45756</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="N34" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="O34" s="21" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="102" customHeight="1">
-      <c r="A35" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="24">
-        <v>45894</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J35" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K35" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L35" s="14"/>
-      <c r="M35" s="6" t="s">
+      <c r="J39" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39" s="8"/>
+      <c r="M39" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="N39" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="N35" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="O35" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="49" customFormat="1" ht="58.3">
-      <c r="A36" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="46">
-        <v>45799</v>
-      </c>
-      <c r="G36" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="H36" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="I36" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="J36" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="K36" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L36" s="45"/>
-      <c r="M36" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="N36" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="O36" s="50" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="58.3">
-      <c r="A37" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F37" s="39">
-        <v>45868</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="J37" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L37" s="11"/>
-      <c r="M37" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="N37" s="11" t="s">
+      <c r="O39" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="O37" s="21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="58.3">
-      <c r="A38" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F38" s="18">
-        <v>45840</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J38" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K38" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L38" s="11"/>
-      <c r="M38" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="N38" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="O38" s="12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="72.900000000000006">
-      <c r="A39" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F39" s="39">
-        <v>45809</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J39" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K39" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L39" s="11"/>
-      <c r="M39" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="N39" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="O39" s="21" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="40" spans="1:15" ht="87.45">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="29"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="26"/>
       <c r="G40" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H40" s="28" t="s">
+      <c r="H40" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="I40" s="28" t="s">
+      <c r="I40" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="M40" s="27"/>
+      <c r="M40" s="24"/>
     </row>
     <row r="41" spans="1:15" ht="58.3">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F41" s="43">
+      <c r="D41" s="8"/>
+      <c r="E41" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="40">
         <v>45855</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G41" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H41" s="11" t="s">
+      <c r="H41" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="I41" s="11" t="s">
+      <c r="I41" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J41" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K41" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L41" s="11"/>
-      <c r="M41" s="20" t="s">
+      <c r="J41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L41" s="8"/>
+      <c r="M41" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="N41" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="O41" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" s="46" customFormat="1">
+      <c r="A42" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="43">
+        <v>45897</v>
+      </c>
+      <c r="G42" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="H42" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="I42" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J42" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42" s="42"/>
+      <c r="M42" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N42" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="O42" s="44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="72.900000000000006">
+      <c r="A43" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="21">
+        <v>45904</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K43" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L43" s="11"/>
+      <c r="M43" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="N43" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="O43" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="58.3">
+      <c r="A44" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="43">
+        <v>45820</v>
+      </c>
+      <c r="G44" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H44" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="I44" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="J44" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K44" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L44" s="42"/>
+      <c r="M44" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N44" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="O44" s="54" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="43.75">
+      <c r="A45" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" s="21">
+        <v>45909</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K45" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L45" s="11"/>
+      <c r="M45" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="N45" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="O45" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N41" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="O41" s="12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" s="49" customFormat="1">
-      <c r="A42" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="B42" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C42" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F42" s="46">
-        <v>45897</v>
-      </c>
-      <c r="G42" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="H42" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="I42" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="J42" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="K42" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L42" s="45"/>
-      <c r="M42" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="N42" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="O42" s="47" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="72.900000000000006">
-      <c r="A43" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="24">
-        <v>45904</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="J43" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K43" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L43" s="14"/>
-      <c r="M43" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="N43" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="O43" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="58.3">
-      <c r="A44" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F44" s="18">
-        <v>45820</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J44" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K44" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L44" s="11"/>
-      <c r="M44" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="N44" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="O44" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="43.75">
-      <c r="A45" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F45" s="24">
-        <v>45909</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="I45" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="J45" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K45" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L45" s="14"/>
-      <c r="M45" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="N45" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="O45" s="7" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Jupyter notebooks and reorganize lab files
- Added Python Basics for Data Science Jupyter notebooks:
  • PY0101EN-1-1-Expressions_Variables.ipynb
  • PY0101EN-1-1-Types.ipynb
  • PY0101EN-4-2-WriteFile.ipynb
  • PY0101EN-5-1-Numpy1D-v2.ipynb

- Added Operating Systems and Security: File Permissions in Linux lab
- Reorganized Pen Testing, Threat Hunting, and Cryptography labs:
  • Final Project Parts 1 and 2
  • Network Protocol Analyzer
  • Port Scanning (NMap GUI and CLI)
  • Practicing Google Dorking
  • Using SNYK to Scan Code Repository
  • Penetration Testing

- Removed duplicate and misplaced versions of these lab files from the Technical Assignments folder

This commit ensures all labs and Jupyter notebooks are properly organized under their respective course folders and ready for portfolio presentation.
</commit_message>
<xml_diff>
--- a/2025_Course_Tracker_Portfolio_NM.xlsx
+++ b/2025_Course_Tracker_Portfolio_NM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\GitHub\Cybersecurity Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE50590-E799-44CC-8D92-92E77F3BE0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28499BC8-8176-418B-A0CD-D05C1DEC083A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="Training_Progress_Tracker" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="200">
   <si>
     <t>Course</t>
   </si>
@@ -549,9 +548,6 @@
   </si>
   <si>
     <t>EdX -IBM</t>
-  </si>
-  <si>
-    <t>Windows &amp; Linux Security Project</t>
   </si>
   <si>
     <t>Upload final project with README</t>
@@ -1793,9 +1789,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45A587F-D2B6-447F-B3AB-8D0BEB05BA92}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -1948,10 +1944,10 @@
         <v>130</v>
       </c>
       <c r="N3" s="51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O3" s="44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="29.5" customHeight="1">
@@ -1991,7 +1987,7 @@
         <v>130</v>
       </c>
       <c r="N4" s="44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O4" s="44" t="s">
         <v>131</v>
@@ -2034,7 +2030,7 @@
         <v>130</v>
       </c>
       <c r="N5" s="44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O5" s="44" t="s">
         <v>131</v>
@@ -2077,7 +2073,7 @@
         <v>130</v>
       </c>
       <c r="N6" s="44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O6" s="44" t="s">
         <v>131</v>
@@ -2120,7 +2116,7 @@
         <v>130</v>
       </c>
       <c r="N7" s="44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O7" s="44" t="s">
         <v>131</v>
@@ -2163,7 +2159,7 @@
         <v>130</v>
       </c>
       <c r="N8" s="51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O8" s="44" t="s">
         <v>134</v>
@@ -2206,7 +2202,7 @@
         <v>130</v>
       </c>
       <c r="N9" s="44" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O9" s="44" t="s">
         <v>135</v>
@@ -2249,7 +2245,7 @@
         <v>130</v>
       </c>
       <c r="N10" s="44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O10" s="44" t="s">
         <v>136</v>
@@ -2315,7 +2311,7 @@
         <v>130</v>
       </c>
       <c r="N12" s="51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O12" s="44"/>
     </row>
@@ -2446,7 +2442,7 @@
         <v>130</v>
       </c>
       <c r="N15" s="44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O15" s="44" t="s">
         <v>141</v>
@@ -2491,7 +2487,7 @@
         <v>130</v>
       </c>
       <c r="N16" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O16" s="44" t="s">
         <v>142</v>
@@ -2536,7 +2532,7 @@
         <v>130</v>
       </c>
       <c r="N17" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O17" s="44" t="s">
         <v>143</v>
@@ -2579,7 +2575,7 @@
         <v>130</v>
       </c>
       <c r="N18" s="44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O18" s="47" t="s">
         <v>151</v>
@@ -2622,7 +2618,7 @@
         <v>130</v>
       </c>
       <c r="N19" s="44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O19" s="47" t="s">
         <v>152</v>
@@ -2665,7 +2661,7 @@
         <v>130</v>
       </c>
       <c r="N20" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O20" s="47" t="s">
         <v>154</v>
@@ -2731,7 +2727,7 @@
         <v>130</v>
       </c>
       <c r="N22" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O22" s="47" t="s">
         <v>155</v>
@@ -2772,7 +2768,7 @@
         <v>130</v>
       </c>
       <c r="N23" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O23" s="47" t="s">
         <v>156</v>
@@ -2780,7 +2776,7 @@
     </row>
     <row r="24" spans="1:15" s="46" customFormat="1" ht="43.75">
       <c r="A24" s="41" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>31</v>
@@ -2815,7 +2811,7 @@
         <v>130</v>
       </c>
       <c r="N24" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O24" s="47" t="s">
         <v>157</v>
@@ -2858,7 +2854,7 @@
         <v>130</v>
       </c>
       <c r="N25" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O25" s="47" t="s">
         <v>158</v>
@@ -2901,7 +2897,7 @@
         <v>130</v>
       </c>
       <c r="N26" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O26" s="47" t="s">
         <v>159</v>
@@ -3030,7 +3026,7 @@
         <v>130</v>
       </c>
       <c r="N29" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O29" s="47" t="s">
         <v>164</v>
@@ -3076,12 +3072,12 @@
         <v>138</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:15" s="46" customFormat="1" ht="72.900000000000006">
       <c r="A31" s="41" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>17</v>
@@ -3116,7 +3112,7 @@
         <v>130</v>
       </c>
       <c r="N31" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O31" s="47" t="s">
         <v>166</v>
@@ -3159,7 +3155,7 @@
         <v>130</v>
       </c>
       <c r="N32" s="44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O32" s="47" t="s">
         <v>153</v>
@@ -3204,55 +3200,55 @@
         <v>130</v>
       </c>
       <c r="N33" s="44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O33" s="44" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="52.3" customHeight="1">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="15">
+      <c r="D34" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="43">
         <v>45756</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="H34" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="H34" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="J34" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8" t="s">
+      <c r="J34" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K34" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L34" s="42"/>
+      <c r="M34" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="N34" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="N34" s="8" t="s">
+      <c r="O34" s="44" t="s">
         <v>173</v>
-      </c>
-      <c r="O34" s="18" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="102" customHeight="1">
@@ -3333,10 +3329,10 @@
         <v>130</v>
       </c>
       <c r="N36" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O36" s="47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="58.3">
@@ -3373,13 +3369,13 @@
       </c>
       <c r="L37" s="8"/>
       <c r="M37" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="N37" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="O37" s="18" t="s">
         <v>179</v>
-      </c>
-      <c r="N37" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="O37" s="18" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="58.3">
@@ -3418,13 +3414,13 @@
       </c>
       <c r="L38" s="8"/>
       <c r="M38" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="N38" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="O38" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="N38" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="O38" s="9" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="72.900000000000006">
@@ -3463,13 +3459,13 @@
       </c>
       <c r="L39" s="8"/>
       <c r="M39" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="N39" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="O39" s="18" t="s">
         <v>183</v>
-      </c>
-      <c r="N39" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="O39" s="18" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="87.45">
@@ -3530,13 +3526,13 @@
       </c>
       <c r="L41" s="8"/>
       <c r="M41" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="N41" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="N41" s="8" t="s">
+      <c r="O41" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="O41" s="9" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="46" customFormat="1">
@@ -3576,7 +3572,7 @@
         <v>130</v>
       </c>
       <c r="N42" s="44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O42" s="44" t="s">
         <v>131</v>
@@ -3622,7 +3618,7 @@
         <v>146</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="58.3">
@@ -3662,10 +3658,10 @@
         <v>130</v>
       </c>
       <c r="N44" s="53" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O44" s="54" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="43.75">
@@ -3708,7 +3704,7 @@
         <v>146</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add course overviews, Cloud Computing final project, Python notebooks, and SQL lab files
- Added Course Overview (Introduction to Cloud Computing)
- Added Final Project: Guess the Capital (Cloud Computing)
- Added Course Overview (Python Basics for Data Science)
- Uploaded Jupyter notebooks for Python Basics (with labs and examples)
- Added SQL lab files for Relational Database Basics:
   • BookShop CREATE/INSERT
   • eBooks MySQL dump
   • eBooks PostgreSQL dump
   • MyAuthors insert script
- Organized files under Cybersecurity Learning > Relational Databases (Basics)
</commit_message>
<xml_diff>
--- a/2025_Course_Tracker_Portfolio_NM.xlsx
+++ b/2025_Course_Tracker_Portfolio_NM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\GitHub\Cybersecurity Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28499BC8-8176-418B-A0CD-D05C1DEC083A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8BBE2C-75B3-443F-AC53-3B2CA8DD5AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="199">
   <si>
     <t>Course</t>
   </si>
@@ -503,9 +503,6 @@
   </si>
   <si>
     <t>Final project with IR plan &amp; DF investigation. Added lab writeups (Cowrie, chain of custody, analysis/reporting). README required</t>
-  </si>
-  <si>
-    <t>Upload the lab/project files (Dockerfile, container config, deployment steps, screenshots)</t>
   </si>
   <si>
     <t>Final project: Deployed app on IBM Cloud (Docker + Code Engine). Include README and screenshots in GitHub. Notes &amp; quizzes cover cloud basics, models, storage, and security.</t>
@@ -572,9 +569,6 @@
   </si>
   <si>
     <t>Completed Google Cybersecurity capstone prep. Included communication plan, reflection, and AI interview practice. Career-prep focus with applied assignments.</t>
-  </si>
-  <si>
-    <t>Final Python Data Analysis Project</t>
   </si>
   <si>
     <t>Completed IBM course. Covered Python basics, data structures, NumPy, Pandas, APIs, web scraping. Final project: applied Python to analyze and manipulate data</t>
@@ -655,6 +649,9 @@
   </si>
   <si>
     <t>Overview done</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> README</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1271,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1314,9 +1311,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1789,9 +1783,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45A587F-D2B6-447F-B3AB-8D0BEB05BA92}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -1808,9 +1802,9 @@
     <col min="10" max="10" width="10.3046875" style="4" customWidth="1"/>
     <col min="11" max="11" width="14.07421875" style="4" customWidth="1"/>
     <col min="12" max="12" width="8.69140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="58.921875" style="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.4609375" style="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42.53515625" style="25" customWidth="1"/>
+    <col min="13" max="13" width="58.921875" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.4609375" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42.53515625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="65.599999999999994" customHeight="1" thickBot="1">
@@ -1832,28 +1826,28 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="26" t="s">
         <v>99</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -1861,7 +1855,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="29.05" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1895,373 +1889,373 @@
         <v>44</v>
       </c>
       <c r="L2" s="7"/>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="46" customFormat="1" ht="102">
-      <c r="A3" s="41" t="s">
+    <row r="3" spans="1:15" s="45" customFormat="1" ht="102">
+      <c r="A3" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="43">
+      <c r="E3" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="42">
         <v>45855</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="45" t="s">
+      <c r="J3" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="41"/>
+      <c r="M3" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N3" s="51" t="s">
-        <v>197</v>
-      </c>
-      <c r="O3" s="44" t="s">
-        <v>196</v>
+      <c r="N3" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="O3" s="43" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="29.5" customHeight="1">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="43">
+      <c r="D4" s="41"/>
+      <c r="E4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="42">
         <v>45875</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="I4" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" s="42"/>
-      <c r="M4" s="44" t="s">
+      <c r="K4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="41"/>
+      <c r="M4" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N4" s="44" t="s">
-        <v>191</v>
-      </c>
-      <c r="O4" s="44" t="s">
+      <c r="N4" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="O4" s="43" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="46" customFormat="1" ht="29.5" customHeight="1">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:15" s="45" customFormat="1" ht="29.5" customHeight="1">
+      <c r="A5" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="43">
+      <c r="D5" s="41"/>
+      <c r="E5" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="42">
         <v>45892</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="45" t="s">
+      <c r="K5" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="41"/>
+      <c r="M5" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="44" t="s">
-        <v>191</v>
-      </c>
-      <c r="O5" s="44" t="s">
+      <c r="N5" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="O5" s="43" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="46" customFormat="1" ht="29.5" customHeight="1">
-      <c r="A6" s="41" t="s">
+    <row r="6" spans="1:15" s="45" customFormat="1" ht="29.5" customHeight="1">
+      <c r="A6" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="43">
+      <c r="D6" s="41"/>
+      <c r="E6" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="42">
         <v>45872</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="42"/>
-      <c r="M6" s="44" t="s">
+      <c r="K6" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="41"/>
+      <c r="M6" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N6" s="44" t="s">
-        <v>191</v>
-      </c>
-      <c r="O6" s="44" t="s">
+      <c r="N6" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="O6" s="43" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="46" customFormat="1" ht="28" customHeight="1">
-      <c r="A7" s="41" t="s">
+    <row r="7" spans="1:15" s="45" customFormat="1" ht="28" customHeight="1">
+      <c r="A7" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="43">
+      <c r="D7" s="41"/>
+      <c r="E7" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="42">
         <v>45866</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="42"/>
-      <c r="M7" s="44" t="s">
+      <c r="K7" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="41"/>
+      <c r="M7" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N7" s="44" t="s">
-        <v>191</v>
-      </c>
-      <c r="O7" s="44" t="s">
+      <c r="N7" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="O7" s="43" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="52" customFormat="1" ht="87.45">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:15" s="51" customFormat="1" ht="87.45">
+      <c r="A8" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="43">
+      <c r="D8" s="41"/>
+      <c r="E8" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="42">
         <v>45817</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="42"/>
-      <c r="M8" s="44" t="s">
+      <c r="J8" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="41"/>
+      <c r="M8" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N8" s="51" t="s">
-        <v>197</v>
-      </c>
-      <c r="O8" s="44" t="s">
+      <c r="N8" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="O8" s="43" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="72.900000000000006">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="43">
+      <c r="D9" s="41"/>
+      <c r="E9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="42">
         <v>45867</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="42"/>
-      <c r="M9" s="44" t="s">
+      <c r="J9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="41"/>
+      <c r="M9" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N9" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="O9" s="44" t="s">
+      <c r="N9" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="O9" s="43" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="46" customFormat="1" ht="43.75">
-      <c r="A10" s="41" t="s">
+    <row r="10" spans="1:15" s="45" customFormat="1" ht="43.75">
+      <c r="A10" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="43">
+      <c r="D10" s="41"/>
+      <c r="E10" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="42">
         <v>45785</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="42" t="s">
+      <c r="I10" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="J10" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42" t="s">
+      <c r="K10" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N10" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="O10" s="44" t="s">
+      <c r="N10" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="O10" s="43" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10" t="s">
         <v>150</v>
@@ -2270,53 +2264,53 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
     </row>
     <row r="12" spans="1:15" ht="30.45" customHeight="1">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="43">
+      <c r="D12" s="41"/>
+      <c r="E12" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="42">
         <v>45808</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="42" t="s">
+      <c r="H12" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="42" t="s">
+      <c r="I12" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42" t="s">
+      <c r="J12" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N12" s="51" t="s">
-        <v>197</v>
-      </c>
-      <c r="O12" s="44"/>
+      <c r="N12" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="O12" s="43"/>
     </row>
     <row r="13" spans="1:15" ht="87.45">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -2331,7 +2325,7 @@
       <c r="E13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="20">
         <v>45748</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -2350,18 +2344,18 @@
         <v>42</v>
       </c>
       <c r="L13" s="11"/>
-      <c r="M13" s="22" t="s">
+      <c r="M13" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="N13" s="22" t="s">
+      <c r="N13" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="O13" s="22" t="s">
+      <c r="O13" s="21" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="29.15">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="32" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -2374,7 +2368,7 @@
       <c r="E14" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="20">
         <v>45900</v>
       </c>
       <c r="G14" s="11" t="s">
@@ -2393,293 +2387,293 @@
         <v>42</v>
       </c>
       <c r="L14" s="11"/>
-      <c r="M14" s="22" t="s">
+      <c r="M14" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="N14" s="22" t="s">
+      <c r="N14" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="O14" s="22" t="s">
+      <c r="O14" s="21" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="46" customFormat="1" ht="43.75">
-      <c r="A15" s="41" t="s">
+    <row r="15" spans="1:15" s="45" customFormat="1" ht="43.75">
+      <c r="A15" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="43">
+      <c r="D15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="42">
         <v>45755</v>
       </c>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="42" t="s">
+      <c r="H15" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="42" t="s">
+      <c r="I15" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="42" t="s">
+      <c r="J15" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L15" s="42"/>
-      <c r="M15" s="44" t="s">
+      <c r="K15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="41"/>
+      <c r="M15" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N15" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="O15" s="44" t="s">
+      <c r="N15" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="O15" s="43" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="46" customFormat="1" ht="43.75">
-      <c r="A16" s="41" t="s">
+    <row r="16" spans="1:15" s="45" customFormat="1" ht="43.75">
+      <c r="A16" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="43">
+      <c r="D16" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="42">
         <v>45799</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="I16" s="42" t="s">
+      <c r="I16" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J16" s="42" t="s">
+      <c r="J16" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L16" s="42"/>
-      <c r="M16" s="44" t="s">
+      <c r="K16" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="41"/>
+      <c r="M16" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N16" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O16" s="44" t="s">
+      <c r="N16" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O16" s="43" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="46" customFormat="1" ht="29.15">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:15" s="45" customFormat="1" ht="29.15">
+      <c r="A17" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="43">
+      <c r="D17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="42">
         <v>45764</v>
       </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="H17" s="42" t="s">
+      <c r="H17" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="42" t="s">
+      <c r="I17" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="42" t="s">
+      <c r="J17" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K17" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L17" s="42"/>
-      <c r="M17" s="44" t="s">
+      <c r="K17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="41"/>
+      <c r="M17" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N17" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O17" s="44" t="s">
+      <c r="N17" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O17" s="43" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="43.75">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="43">
+      <c r="D18" s="41"/>
+      <c r="E18" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="42">
         <v>45791</v>
       </c>
-      <c r="G18" s="42" t="s">
+      <c r="G18" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="42" t="s">
+      <c r="H18" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="42" t="s">
+      <c r="I18" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42" t="s">
+      <c r="J18" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N18" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="O18" s="47" t="s">
+      <c r="N18" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="O18" s="46" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="43.75">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="43">
+      <c r="D19" s="41"/>
+      <c r="E19" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="42">
         <v>45779</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="42" t="s">
+      <c r="I19" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42" t="s">
+      <c r="J19" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N19" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="O19" s="47" t="s">
+      <c r="N19" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="O19" s="46" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="46" customFormat="1" ht="87.45">
-      <c r="A20" s="41" t="s">
+    <row r="20" spans="1:15" s="45" customFormat="1" ht="87.45">
+      <c r="A20" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="43">
+      <c r="D20" s="41"/>
+      <c r="E20" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="42">
         <v>45902</v>
       </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="42" t="s">
+      <c r="H20" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="42" t="s">
+      <c r="I20" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="J20" s="42" t="s">
+      <c r="J20" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K20" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20" s="42"/>
-      <c r="M20" s="44" t="s">
+      <c r="K20" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="41"/>
+      <c r="M20" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N20" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O20" s="47" t="s">
+      <c r="N20" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O20" s="46" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="34"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="4" t="s">
         <v>148</v>
       </c>
@@ -2690,221 +2684,221 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="46" customFormat="1" ht="29.15">
-      <c r="A22" s="41" t="s">
+    <row r="22" spans="1:15" s="45" customFormat="1" ht="29.15">
+      <c r="A22" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="43">
+      <c r="D22" s="41"/>
+      <c r="E22" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="42">
         <v>45797</v>
       </c>
-      <c r="G22" s="42" t="s">
+      <c r="G22" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="42" t="s">
+      <c r="H22" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="I22" s="42" t="s">
+      <c r="I22" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="42" t="s">
+      <c r="J22" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L22" s="42"/>
-      <c r="M22" s="44" t="s">
+      <c r="K22" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" s="41"/>
+      <c r="M22" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N22" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O22" s="47" t="s">
+      <c r="N22" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O22" s="46" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="46" customFormat="1" ht="58.3">
-      <c r="A23" s="41" t="s">
+    <row r="23" spans="1:15" s="45" customFormat="1" ht="58.3">
+      <c r="A23" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="48">
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="47">
         <v>45909</v>
       </c>
-      <c r="G23" s="42" t="s">
+      <c r="G23" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="42" t="s">
+      <c r="H23" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="I23" s="42" t="s">
+      <c r="I23" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="42" t="s">
+      <c r="J23" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K23" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L23" s="42"/>
-      <c r="M23" s="44" t="s">
+      <c r="K23" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" s="41"/>
+      <c r="M23" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N23" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O23" s="47" t="s">
+      <c r="N23" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O23" s="46" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="46" customFormat="1" ht="43.75">
-      <c r="A24" s="41" t="s">
-        <v>194</v>
-      </c>
-      <c r="B24" s="42" t="s">
+    <row r="24" spans="1:15" s="45" customFormat="1" ht="43.75">
+      <c r="A24" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="43">
+      <c r="D24" s="41"/>
+      <c r="E24" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="42">
         <v>45907</v>
       </c>
-      <c r="G24" s="42" t="s">
+      <c r="G24" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="42" t="s">
+      <c r="H24" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="I24" s="42" t="s">
+      <c r="I24" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="J24" s="42" t="s">
+      <c r="J24" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L24" s="42"/>
-      <c r="M24" s="44" t="s">
+      <c r="K24" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L24" s="41"/>
+      <c r="M24" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N24" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O24" s="47" t="s">
+      <c r="N24" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O24" s="46" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="46" customFormat="1" ht="72.900000000000006">
-      <c r="A25" s="41" t="s">
+    <row r="25" spans="1:15" s="45" customFormat="1" ht="72.900000000000006">
+      <c r="A25" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="43">
+      <c r="D25" s="41"/>
+      <c r="E25" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="42">
         <v>45904</v>
       </c>
-      <c r="G25" s="42" t="s">
+      <c r="G25" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="42" t="s">
+      <c r="H25" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="I25" s="42" t="s">
+      <c r="I25" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="42" t="s">
+      <c r="J25" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K25" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L25" s="42"/>
-      <c r="M25" s="44" t="s">
+      <c r="K25" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L25" s="41"/>
+      <c r="M25" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N25" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O25" s="47" t="s">
+      <c r="N25" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O25" s="46" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="46" customFormat="1" ht="72.900000000000006">
-      <c r="A26" s="41" t="s">
+    <row r="26" spans="1:15" s="45" customFormat="1" ht="72.900000000000006">
+      <c r="A26" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="43">
+      <c r="D26" s="41"/>
+      <c r="E26" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="42">
         <v>45905</v>
       </c>
-      <c r="G26" s="42" t="s">
+      <c r="G26" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="H26" s="42" t="s">
+      <c r="H26" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="I26" s="42" t="s">
+      <c r="I26" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="J26" s="42" t="s">
+      <c r="J26" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K26" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="42"/>
-      <c r="M26" s="44" t="s">
+      <c r="K26" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="41"/>
+      <c r="M26" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N26" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O26" s="47" t="s">
+      <c r="N26" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O26" s="46" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="43.75">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="11" t="s">
@@ -2917,7 +2911,7 @@
       <c r="E27" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="35">
+      <c r="F27" s="34">
         <v>45872</v>
       </c>
       <c r="G27" s="11" t="s">
@@ -2936,10 +2930,10 @@
         <v>42</v>
       </c>
       <c r="L27" s="11"/>
-      <c r="M27" s="29" t="s">
+      <c r="M27" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="N27" s="22" t="s">
+      <c r="N27" s="21" t="s">
         <v>138</v>
       </c>
       <c r="O27" s="12" t="s">
@@ -2947,93 +2941,93 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="58.3">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="15">
+      <c r="D28" s="41"/>
+      <c r="E28" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="42">
         <v>45790</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L28" s="8"/>
-      <c r="M28" s="18" t="s">
+      <c r="J28" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="41"/>
+      <c r="M28" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="N28" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="O28" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="N28" s="9" t="s">
+    </row>
+    <row r="29" spans="1:15" s="45" customFormat="1" ht="58.3">
+      <c r="A29" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="42">
+        <v>45819</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="I29" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="J29" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="K29" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29" s="41"/>
+      <c r="M29" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="N29" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O29" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="O28" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" s="46" customFormat="1" ht="58.3">
-      <c r="A29" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="43">
-        <v>45819</v>
-      </c>
-      <c r="G29" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="I29" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="J29" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="K29" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L29" s="42"/>
-      <c r="M29" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="N29" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O29" s="47" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="30" spans="1:15" ht="43.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="32" t="s">
         <v>109</v>
       </c>
       <c r="B30" s="11" t="s">
@@ -3046,7 +3040,7 @@
       <c r="E30" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="20">
         <v>45902</v>
       </c>
       <c r="G30" s="11" t="s">
@@ -3065,194 +3059,194 @@
         <v>42</v>
       </c>
       <c r="L30" s="11"/>
-      <c r="M30" s="22" t="s">
+      <c r="M30" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="N30" s="22" t="s">
+      <c r="N30" s="21" t="s">
         <v>138</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="46" customFormat="1" ht="72.900000000000006">
-      <c r="A31" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="B31" s="42" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="45" customFormat="1" ht="72.900000000000006">
+      <c r="A31" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B31" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="43">
+      <c r="D31" s="41"/>
+      <c r="E31" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="42">
         <v>45744</v>
       </c>
-      <c r="G31" s="42" t="s">
+      <c r="G31" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="H31" s="42" t="s">
+      <c r="H31" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="I31" s="42" t="s">
+      <c r="I31" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="J31" s="42" t="s">
+      <c r="J31" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K31" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L31" s="42"/>
-      <c r="M31" s="44" t="s">
+      <c r="K31" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31" s="41"/>
+      <c r="M31" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N31" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O31" s="47" t="s">
-        <v>166</v>
+      <c r="N31" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O31" s="46" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="43.75">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="43">
+      <c r="D32" s="41"/>
+      <c r="E32" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="42">
         <v>45780</v>
       </c>
-      <c r="G32" s="42" t="s">
+      <c r="G32" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="H32" s="42" t="s">
+      <c r="H32" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="I32" s="42" t="s">
+      <c r="I32" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K32" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42" t="s">
+      <c r="J32" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N32" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="O32" s="47" t="s">
+      <c r="N32" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="O32" s="46" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="46" customFormat="1" ht="43.75">
-      <c r="A33" s="41" t="s">
+    <row r="33" spans="1:15" s="45" customFormat="1" ht="43.75">
+      <c r="A33" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="43">
+      <c r="D33" s="41"/>
+      <c r="E33" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="42">
         <v>45903</v>
       </c>
-      <c r="G33" s="42" t="s">
+      <c r="G33" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="42" t="s">
+      <c r="H33" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="I33" s="42" t="s">
+      <c r="I33" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J33" s="42" t="s">
+      <c r="J33" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K33" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L33" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="M33" s="44" t="s">
+      <c r="K33" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L33" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="M33" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N33" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="O33" s="44" t="s">
+      <c r="N33" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="O33" s="43" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="52.3" customHeight="1">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="C34" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="42">
+        <v>45756</v>
+      </c>
+      <c r="G34" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="H34" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="I34" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="J34" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K34" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N34" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="43">
-        <v>45756</v>
-      </c>
-      <c r="G34" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="H34" s="42" t="s">
-        <v>175</v>
-      </c>
-      <c r="I34" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J34" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K34" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="N34" s="42" t="s">
+      <c r="O34" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="O34" s="44" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="35" spans="1:15" ht="102" customHeight="1">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="32" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -3263,7 +3257,7 @@
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="21">
+      <c r="F35" s="20">
         <v>45894</v>
       </c>
       <c r="G35" s="11" t="s">
@@ -3283,60 +3277,60 @@
       </c>
       <c r="L35" s="11"/>
       <c r="M35" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="N35" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="N35" s="12" t="s">
+      <c r="O35" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="O35" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="46" customFormat="1" ht="58.3">
-      <c r="A36" s="49" t="s">
+    </row>
+    <row r="36" spans="1:15" s="45" customFormat="1" ht="58.3">
+      <c r="A36" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="43">
+      <c r="D36" s="49"/>
+      <c r="E36" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="42">
         <v>45799</v>
       </c>
-      <c r="G36" s="42" t="s">
+      <c r="G36" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H36" s="42" t="s">
+      <c r="H36" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="I36" s="42" t="s">
+      <c r="I36" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J36" s="42" t="s">
+      <c r="J36" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L36" s="42"/>
-      <c r="M36" s="44" t="s">
+      <c r="K36" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L36" s="41"/>
+      <c r="M36" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N36" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="O36" s="47" t="s">
-        <v>176</v>
+      <c r="N36" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="O36" s="46" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="58.3">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -3349,7 +3343,7 @@
       <c r="E37" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F37" s="36">
+      <c r="F37" s="35">
         <v>45868</v>
       </c>
       <c r="G37" s="8" t="s">
@@ -3368,78 +3362,78 @@
         <v>42</v>
       </c>
       <c r="L37" s="8"/>
-      <c r="M37" s="18" t="s">
+      <c r="M37" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N37" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="O37" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="N37" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="O37" s="18" t="s">
+    </row>
+    <row r="38" spans="1:15" ht="58.3">
+      <c r="A38" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="42">
+        <v>45840</v>
+      </c>
+      <c r="G38" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="H38" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="J38" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L38" s="41"/>
+      <c r="M38" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="N38" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="O38" s="46" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="58.3">
-      <c r="A38" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="8" t="s">
+    <row r="39" spans="1:15" ht="72.900000000000006">
+      <c r="A39" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C39" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F38" s="15">
-        <v>45840</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L38" s="8"/>
-      <c r="M38" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="N38" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="O38" s="9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="72.900000000000006">
-      <c r="A39" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="F39" s="36">
+      <c r="D39" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="35">
         <v>45809</v>
       </c>
       <c r="G39" s="8" t="s">
@@ -3458,42 +3452,42 @@
         <v>42</v>
       </c>
       <c r="L39" s="8"/>
-      <c r="M39" s="18" t="s">
-        <v>182</v>
+      <c r="M39" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="O39" s="18" t="s">
-        <v>183</v>
+        <v>171</v>
+      </c>
+      <c r="O39" s="17" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="87.45">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="26"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="25"/>
       <c r="G40" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H40" s="25" t="s">
+      <c r="H40" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="I40" s="25" t="s">
+      <c r="I40" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="M40" s="24"/>
+      <c r="M40" s="23"/>
     </row>
     <row r="41" spans="1:15" ht="58.3">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="30" t="s">
         <v>14</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -3503,10 +3497,10 @@
         <v>8</v>
       </c>
       <c r="D41" s="8"/>
-      <c r="E41" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="F41" s="40">
+      <c r="E41" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="39">
         <v>45855</v>
       </c>
       <c r="G41" s="8" t="s">
@@ -3525,61 +3519,61 @@
         <v>42</v>
       </c>
       <c r="L41" s="8"/>
-      <c r="M41" s="17" t="s">
+      <c r="M41" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="N41" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="O41" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="N41" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="O41" s="9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" s="46" customFormat="1">
-      <c r="A42" s="41" t="s">
+    </row>
+    <row r="42" spans="1:15" s="45" customFormat="1">
+      <c r="A42" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="42" t="s">
+      <c r="C42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F42" s="43">
+      <c r="D42" s="41"/>
+      <c r="E42" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="42">
         <v>45897</v>
       </c>
-      <c r="G42" s="42" t="s">
+      <c r="G42" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H42" s="42" t="s">
+      <c r="H42" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="I42" s="42" t="s">
+      <c r="I42" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="J42" s="42" t="s">
+      <c r="J42" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K42" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L42" s="42"/>
-      <c r="M42" s="44" t="s">
+      <c r="K42" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42" s="41"/>
+      <c r="M42" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N42" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="O42" s="44" t="s">
+      <c r="N42" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="O42" s="43" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="72.900000000000006">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="32" t="s">
         <v>111</v>
       </c>
       <c r="B43" s="11" t="s">
@@ -3592,7 +3586,7 @@
       <c r="E43" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F43" s="21">
+      <c r="F43" s="20">
         <v>45904</v>
       </c>
       <c r="G43" s="11" t="s">
@@ -3611,61 +3605,61 @@
         <v>42</v>
       </c>
       <c r="L43" s="11"/>
-      <c r="M43" s="29" t="s">
+      <c r="M43" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="N43" s="22" t="s">
+      <c r="N43" s="21" t="s">
         <v>146</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="58.3">
-      <c r="A44" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="B44" s="42" t="s">
+      <c r="A44" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C44" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F44" s="43">
+      <c r="D44" s="41"/>
+      <c r="E44" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="42">
         <v>45820</v>
       </c>
-      <c r="G44" s="42" t="s">
+      <c r="G44" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="H44" s="42" t="s">
+      <c r="H44" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="I44" s="42" t="s">
+      <c r="I44" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J44" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K44" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L44" s="42"/>
-      <c r="M44" s="44" t="s">
+      <c r="J44" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K44" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L44" s="41"/>
+      <c r="M44" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="N44" s="53" t="s">
-        <v>199</v>
-      </c>
-      <c r="O44" s="54" t="s">
-        <v>187</v>
+      <c r="N44" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="O44" s="53" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="43.75">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="32" t="s">
         <v>113</v>
       </c>
       <c r="B45" s="11" t="s">
@@ -3678,7 +3672,7 @@
       <c r="E45" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F45" s="21">
+      <c r="F45" s="20">
         <v>45909</v>
       </c>
       <c r="G45" s="11" t="s">
@@ -3697,14 +3691,14 @@
         <v>42</v>
       </c>
       <c r="L45" s="11"/>
-      <c r="M45" s="29" t="s">
+      <c r="M45" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="N45" s="22" t="s">
+      <c r="N45" s="21" t="s">
         <v>146</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added course materials and lab documents for Relational Database Basics.
This push includes the final project and supporting lab files from the Relational Database Basics course. Files cover database design and implementation, normalization, keys and constraints, ERDs, and data loading in both PostgreSQL (pgAdmin) and MySQL (phpMyAdmin). These resources document schema creation, normalization, and cross-platform database management as part of the training.
</commit_message>
<xml_diff>
--- a/2025_Course_Tracker_Portfolio_NM.xlsx
+++ b/2025_Course_Tracker_Portfolio_NM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\GitHub\Cybersecurity Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8BBE2C-75B3-443F-AC53-3B2CA8DD5AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E12F41-4B2B-4F42-A976-0EE7A07EE66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="198">
   <si>
     <t>Course</t>
   </si>
@@ -572,9 +572,6 @@
   </si>
   <si>
     <t>Completed IBM course. Covered Python basics, data structures, NumPy, Pandas, APIs, web scraping. Final project: applied Python to analyze and manipulate data</t>
-  </si>
-  <si>
-    <t>Relational Database Final Project (ERD, normalization, schema, sample queries)</t>
   </si>
   <si>
     <t>Completed IBM course. Covered SQL basics, Db2/MySQL/PostgreSQL, ERDs, normalization, constraints. Final project: design relational database with ERD, normalized tables, views, and data load.</t>
@@ -1271,7 +1268,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1374,12 +1371,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="36" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1783,9 +1774,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45A587F-D2B6-447F-B3AB-8D0BEB05BA92}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N28" sqref="N28"/>
+      <selection pane="topRight" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -1899,349 +1890,349 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="45" customFormat="1" ht="102">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:15" s="43" customFormat="1" ht="102">
+      <c r="A3" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="42">
+      <c r="E3" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="40">
         <v>45855</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="44" t="s">
+      <c r="J3" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="39"/>
+      <c r="M3" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="N3" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="O3" s="43" t="s">
+      <c r="N3" s="48" t="s">
         <v>194</v>
       </c>
+      <c r="O3" s="41" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="4" spans="1:15" ht="29.5" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="42">
+      <c r="D4" s="39"/>
+      <c r="E4" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="40">
         <v>45875</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="43" t="s">
+      <c r="K4" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="39"/>
+      <c r="M4" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N4" s="43" t="s">
+      <c r="N4" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="O4" s="41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="43" customFormat="1" ht="29.5" customHeight="1">
+      <c r="A5" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="40">
+        <v>45892</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="39"/>
+      <c r="M5" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="N5" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="O5" s="41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="43" customFormat="1" ht="29.5" customHeight="1">
+      <c r="A6" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="40">
+        <v>45872</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="39"/>
+      <c r="M6" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N6" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="O6" s="41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="43" customFormat="1" ht="28" customHeight="1">
+      <c r="A7" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="40">
+        <v>45866</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="39"/>
+      <c r="M7" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N7" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="O7" s="41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="49" customFormat="1" ht="87.45">
+      <c r="A8" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="40">
+        <v>45817</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="39"/>
+      <c r="M8" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N8" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="72.900000000000006">
+      <c r="A9" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="40">
+        <v>45867</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="39"/>
+      <c r="M9" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N9" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="O9" s="41" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="43" customFormat="1" ht="43.75">
+      <c r="A10" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="40">
+        <v>45785</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="N10" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="O4" s="43" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="45" customFormat="1" ht="29.5" customHeight="1">
-      <c r="A5" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="42">
-        <v>45892</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="I5" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="N5" s="43" t="s">
-        <v>189</v>
-      </c>
-      <c r="O5" s="43" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="45" customFormat="1" ht="29.5" customHeight="1">
-      <c r="A6" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="42">
-        <v>45872</v>
-      </c>
-      <c r="G6" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="41"/>
-      <c r="M6" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="N6" s="43" t="s">
-        <v>189</v>
-      </c>
-      <c r="O6" s="43" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="45" customFormat="1" ht="28" customHeight="1">
-      <c r="A7" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="42">
-        <v>45866</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="41"/>
-      <c r="M7" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="N7" s="43" t="s">
-        <v>189</v>
-      </c>
-      <c r="O7" s="43" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="51" customFormat="1" ht="87.45">
-      <c r="A8" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="42">
-        <v>45817</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="41"/>
-      <c r="M8" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="N8" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="O8" s="43" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="72.900000000000006">
-      <c r="A9" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="42">
-        <v>45867</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="I9" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="N9" s="43" t="s">
-        <v>195</v>
-      </c>
-      <c r="O9" s="43" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="45" customFormat="1" ht="43.75">
-      <c r="A10" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="42">
-        <v>45785</v>
-      </c>
-      <c r="G10" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="N10" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="O10" s="43" t="s">
+      <c r="O10" s="41" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2269,45 +2260,45 @@
       <c r="O11" s="19"/>
     </row>
     <row r="12" spans="1:15" ht="30.45" customHeight="1">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="42">
+      <c r="D12" s="39"/>
+      <c r="E12" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="40">
         <v>45808</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="41" t="s">
+      <c r="H12" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="41" t="s">
+      <c r="I12" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41" t="s">
+      <c r="J12" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="N12" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="O12" s="43"/>
+      <c r="N12" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="O12" s="41"/>
     </row>
     <row r="13" spans="1:15" ht="87.45">
       <c r="A13" s="32" t="s">
@@ -2397,267 +2388,267 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="45" customFormat="1" ht="43.75">
-      <c r="A15" s="40" t="s">
+    <row r="15" spans="1:15" s="43" customFormat="1" ht="43.75">
+      <c r="A15" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="42">
+      <c r="D15" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="40">
         <v>45755</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L15" s="41"/>
-      <c r="M15" s="43" t="s">
+      <c r="K15" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="39"/>
+      <c r="M15" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N15" s="43" t="s">
+      <c r="N15" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="O15" s="41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="43" customFormat="1" ht="43.75">
+      <c r="A16" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="40">
+        <v>45799</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="39"/>
+      <c r="M16" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N16" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="O15" s="43" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="45" customFormat="1" ht="43.75">
-      <c r="A16" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="41" t="s">
+      <c r="O16" s="41" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="43" customFormat="1" ht="29.15">
+      <c r="A17" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C17" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="42">
-        <v>45799</v>
-      </c>
-      <c r="G16" s="41" t="s">
+      <c r="D17" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="40">
+        <v>45764</v>
+      </c>
+      <c r="G17" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H16" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" s="41" t="s">
+      <c r="H17" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J16" s="41" t="s">
+      <c r="J17" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L16" s="41"/>
-      <c r="M16" s="43" t="s">
+      <c r="K17" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="39"/>
+      <c r="M17" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N16" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O16" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="45" customFormat="1" ht="29.15">
-      <c r="A17" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="41" t="s">
+      <c r="N17" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O17" s="41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="43.75">
+      <c r="A18" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="40">
+        <v>45791</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="N18" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="O18" s="44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="43.75">
+      <c r="A19" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="40">
+        <v>45779</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="N19" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="O19" s="44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="43" customFormat="1" ht="87.45">
+      <c r="A20" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="42">
-        <v>45764</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="41" t="s">
+      <c r="D20" s="39"/>
+      <c r="E20" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="40">
+        <v>45902</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K17" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L17" s="41"/>
-      <c r="M17" s="43" t="s">
+      <c r="K20" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="39"/>
+      <c r="M20" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N17" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O17" s="43" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="43.75">
-      <c r="A18" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="42">
-        <v>45791</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="N18" s="43" t="s">
-        <v>196</v>
-      </c>
-      <c r="O18" s="46" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="43.75">
-      <c r="A19" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="42">
-        <v>45779</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="N19" s="43" t="s">
-        <v>196</v>
-      </c>
-      <c r="O19" s="46" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="45" customFormat="1" ht="87.45">
-      <c r="A20" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="42">
-        <v>45902</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="J20" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K20" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20" s="41"/>
-      <c r="M20" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="N20" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O20" s="46" t="s">
+      <c r="N20" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O20" s="44" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2684,216 +2675,216 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="45" customFormat="1" ht="29.15">
-      <c r="A22" s="40" t="s">
+    <row r="22" spans="1:15" s="43" customFormat="1" ht="29.15">
+      <c r="A22" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="42">
+      <c r="D22" s="39"/>
+      <c r="E22" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="40">
         <v>45797</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G22" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="I22" s="41" t="s">
+      <c r="I22" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L22" s="41"/>
-      <c r="M22" s="43" t="s">
+      <c r="K22" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" s="39"/>
+      <c r="M22" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N22" s="43" t="s">
+      <c r="N22" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O22" s="44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="43" customFormat="1" ht="58.3">
+      <c r="A23" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="45">
+        <v>45909</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="K23" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" s="39"/>
+      <c r="M23" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N23" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O23" s="44" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="43" customFormat="1" ht="43.75">
+      <c r="A24" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="O22" s="46" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" s="45" customFormat="1" ht="58.3">
-      <c r="A23" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="41" t="s">
+      <c r="B24" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C24" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="47">
-        <v>45909</v>
-      </c>
-      <c r="G23" s="41" t="s">
+      <c r="D24" s="39"/>
+      <c r="E24" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="40">
+        <v>45907</v>
+      </c>
+      <c r="G24" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="I23" s="41" t="s">
+      <c r="H24" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L24" s="39"/>
+      <c r="M24" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N24" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O24" s="44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="43" customFormat="1" ht="72.900000000000006">
+      <c r="A25" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="40">
+        <v>45904</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="41" t="s">
+      <c r="J25" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K23" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L23" s="41"/>
-      <c r="M23" s="43" t="s">
+      <c r="K25" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L25" s="39"/>
+      <c r="M25" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N23" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O23" s="46" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" s="45" customFormat="1" ht="43.75">
-      <c r="A24" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="41" t="s">
+      <c r="N25" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O25" s="44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="43" customFormat="1" ht="72.900000000000006">
+      <c r="A26" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="42">
-        <v>45907</v>
-      </c>
-      <c r="G24" s="41" t="s">
+      <c r="D26" s="39"/>
+      <c r="E26" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="40">
+        <v>45905</v>
+      </c>
+      <c r="G26" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="I24" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="J24" s="41" t="s">
+      <c r="H26" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I26" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L24" s="41"/>
-      <c r="M24" s="43" t="s">
+      <c r="K26" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="39"/>
+      <c r="M26" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N24" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O24" s="46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" s="45" customFormat="1" ht="72.900000000000006">
-      <c r="A25" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="42">
-        <v>45904</v>
-      </c>
-      <c r="G25" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="I25" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K25" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L25" s="41"/>
-      <c r="M25" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="N25" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O25" s="46" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="45" customFormat="1" ht="72.900000000000006">
-      <c r="A26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="42">
-        <v>45905</v>
-      </c>
-      <c r="G26" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="H26" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="I26" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K26" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="41"/>
-      <c r="M26" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="N26" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O26" s="46" t="s">
+      <c r="N26" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O26" s="44" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2941,88 +2932,88 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="58.3">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="42">
+      <c r="D28" s="39"/>
+      <c r="E28" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="40">
         <v>45790</v>
       </c>
-      <c r="G28" s="41" t="s">
+      <c r="G28" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="41" t="s">
+      <c r="H28" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="41" t="s">
+      <c r="I28" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="J28" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K28" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L28" s="41"/>
-      <c r="M28" s="43" t="s">
+      <c r="J28" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="39"/>
+      <c r="M28" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N28" s="46" t="s">
+      <c r="N28" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="O28" s="46" t="s">
+      <c r="O28" s="44" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="45" customFormat="1" ht="58.3">
-      <c r="A29" s="40" t="s">
+    <row r="29" spans="1:15" s="43" customFormat="1" ht="58.3">
+      <c r="A29" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="42">
+      <c r="D29" s="39"/>
+      <c r="E29" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="40">
         <v>45819</v>
       </c>
-      <c r="G29" s="41" t="s">
+      <c r="G29" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H29" s="41" t="s">
+      <c r="H29" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="I29" s="41" t="s">
+      <c r="I29" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="J29" s="41" t="s">
+      <c r="J29" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L29" s="41"/>
-      <c r="M29" s="43" t="s">
+      <c r="K29" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29" s="39"/>
+      <c r="M29" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N29" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O29" s="46" t="s">
+      <c r="N29" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O29" s="44" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3066,182 +3057,182 @@
         <v>138</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="45" customFormat="1" ht="72.900000000000006">
-      <c r="A31" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="B31" s="41" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="43" customFormat="1" ht="72.900000000000006">
+      <c r="A31" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="B31" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="42">
+      <c r="D31" s="39"/>
+      <c r="E31" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="40">
         <v>45744</v>
       </c>
-      <c r="G31" s="41" t="s">
+      <c r="G31" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H31" s="41" t="s">
+      <c r="H31" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="I31" s="41" t="s">
+      <c r="I31" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="J31" s="41" t="s">
+      <c r="J31" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K31" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L31" s="41"/>
-      <c r="M31" s="43" t="s">
+      <c r="K31" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31" s="39"/>
+      <c r="M31" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N31" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O31" s="46" t="s">
+      <c r="N31" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O31" s="44" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="43.75">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="42">
+      <c r="D32" s="39"/>
+      <c r="E32" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="40">
         <v>45780</v>
       </c>
-      <c r="G32" s="41" t="s">
+      <c r="G32" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="H32" s="41" t="s">
+      <c r="H32" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="I32" s="41" t="s">
+      <c r="I32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K32" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41" t="s">
+      <c r="J32" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="N32" s="43" t="s">
-        <v>196</v>
-      </c>
-      <c r="O32" s="46" t="s">
+      <c r="N32" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="O32" s="44" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="45" customFormat="1" ht="43.75">
-      <c r="A33" s="40" t="s">
+    <row r="33" spans="1:15" s="43" customFormat="1" ht="43.75">
+      <c r="A33" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="42">
+      <c r="D33" s="39"/>
+      <c r="E33" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="40">
         <v>45903</v>
       </c>
-      <c r="G33" s="41" t="s">
+      <c r="G33" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H33" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="I33" s="41" t="s">
+      <c r="I33" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J33" s="41" t="s">
+      <c r="J33" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K33" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L33" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="M33" s="43" t="s">
+      <c r="K33" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L33" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="M33" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N33" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="O33" s="43" t="s">
+      <c r="N33" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="O33" s="41" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="52.3" customHeight="1">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="42">
+      <c r="D34" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="40">
         <v>45756</v>
       </c>
-      <c r="G34" s="41" t="s">
+      <c r="G34" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="H34" s="41" t="s">
+      <c r="H34" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J34" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K34" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L34" s="41"/>
-      <c r="M34" s="41" t="s">
+      <c r="J34" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K34" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="N34" s="41" t="s">
+      <c r="N34" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="O34" s="43" t="s">
+      <c r="O34" s="41" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3286,46 +3277,46 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="45" customFormat="1" ht="58.3">
-      <c r="A36" s="48" t="s">
+    <row r="36" spans="1:15" s="43" customFormat="1" ht="58.3">
+      <c r="A36" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="42">
+      <c r="D36" s="47"/>
+      <c r="E36" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="40">
         <v>45799</v>
       </c>
-      <c r="G36" s="41" t="s">
+      <c r="G36" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H36" s="41" t="s">
+      <c r="H36" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="I36" s="41" t="s">
+      <c r="I36" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J36" s="41" t="s">
+      <c r="J36" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L36" s="41"/>
-      <c r="M36" s="43" t="s">
+      <c r="K36" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L36" s="39"/>
+      <c r="M36" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N36" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="O36" s="46" t="s">
+      <c r="N36" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="O36" s="44" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3373,93 +3364,93 @@
       </c>
     </row>
     <row r="38" spans="1:15" ht="58.3">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F38" s="42">
+      <c r="D38" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="40">
         <v>45840</v>
       </c>
-      <c r="G38" s="41" t="s">
+      <c r="G38" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H38" s="41" t="s">
+      <c r="H38" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="I38" s="41" t="s">
+      <c r="I38" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J38" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K38" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L38" s="41"/>
-      <c r="M38" s="43" t="s">
+      <c r="J38" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L38" s="39"/>
+      <c r="M38" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N38" s="41" t="s">
-        <v>198</v>
-      </c>
-      <c r="O38" s="46" t="s">
+      <c r="N38" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="O38" s="44" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="72.900000000000006">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="F39" s="35">
+      <c r="D39" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="45">
         <v>45809</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I39" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J39" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L39" s="8"/>
-      <c r="M39" s="17" t="s">
+      <c r="J39" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39" s="39"/>
+      <c r="M39" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N39" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="O39" s="41" t="s">
         <v>180</v>
-      </c>
-      <c r="N39" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="87.45">
@@ -3497,10 +3488,10 @@
         <v>8</v>
       </c>
       <c r="D41" s="8"/>
-      <c r="E41" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="F41" s="39">
+      <c r="E41" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="37">
         <v>45855</v>
       </c>
       <c r="G41" s="8" t="s">
@@ -3520,55 +3511,55 @@
       </c>
       <c r="L41" s="8"/>
       <c r="M41" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="N41" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="N41" s="8" t="s">
+      <c r="O41" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="O41" s="9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" s="45" customFormat="1">
-      <c r="A42" s="40" t="s">
+    </row>
+    <row r="42" spans="1:15" s="43" customFormat="1">
+      <c r="A42" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F42" s="42">
+      <c r="D42" s="39"/>
+      <c r="E42" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="40">
         <v>45897</v>
       </c>
-      <c r="G42" s="41" t="s">
+      <c r="G42" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I42" s="41" t="s">
+      <c r="I42" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="J42" s="41" t="s">
+      <c r="J42" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K42" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L42" s="41"/>
-      <c r="M42" s="43" t="s">
+      <c r="K42" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42" s="39"/>
+      <c r="M42" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N42" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="O42" s="43" t="s">
+      <c r="N42" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="O42" s="41" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3612,50 +3603,50 @@
         <v>146</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="58.3">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F44" s="42">
+      <c r="D44" s="39"/>
+      <c r="E44" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="40">
         <v>45820</v>
       </c>
-      <c r="G44" s="41" t="s">
+      <c r="G44" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H44" s="41" t="s">
+      <c r="H44" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="I44" s="41" t="s">
+      <c r="I44" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J44" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K44" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L44" s="41"/>
-      <c r="M44" s="43" t="s">
+      <c r="J44" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K44" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L44" s="39"/>
+      <c r="M44" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N44" s="52" t="s">
-        <v>197</v>
-      </c>
-      <c r="O44" s="53" t="s">
-        <v>185</v>
+      <c r="N44" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="O44" s="51" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="43.75">
@@ -3698,7 +3689,7 @@
         <v>146</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bulk Update: Writing Materials, Technical Assignments, and README Sync
Renamed folders and synced naming conventions across GitHub and desktop (Technical Writing → Technical Communication)

Added and revised README.md files for all writing and technical assignment folders

Added course overviews for:

Pen Testing, Threat Hunting, and Cryptography

Incident Response and Digital Forensics

Connect and Protect

Updated Visual Aids README to match actual contents (phishing stats, home inventory, visual diagrams)

Added writing course content for:

Technical Writing Intro

Technical Communication

Synced all file modifications, new uploads, and course tracker Excel draft
</commit_message>
<xml_diff>
--- a/2025_Course_Tracker_Portfolio_NM.xlsx
+++ b/2025_Course_Tracker_Portfolio_NM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\GitHub\Cybersecurity Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6E9734-0475-45B7-98C0-FC7DA8117D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF55B09-EB69-4443-860D-4B4D2353DCDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
   </bookViews>
@@ -1722,9 +1722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45A587F-D2B6-447F-B3AB-8D0BEB05BA92}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C6" sqref="C6"/>
+      <selection pane="topRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>

</xml_diff>

<commit_message>
Finalize resume, cover letter, and portfolio updates
- Added Natascha_Martin_Public_Resume_2025.pdf (public-safe resume version)
- Added Natascha_Martin_GitHub_Cover_Letter_2025.pdf (core cover letter template)
- Updated README.md with featured projects, badges, and contact line
- Confirmed repo topics/tags (20 max) for cybersecurity, GRC, IR, forensics
- Uploaded course tracker (2025 progress record)
- Cleaned and finalized portfolio for recruiter/job board readiness
</commit_message>
<xml_diff>
--- a/2025_Course_Tracker_Portfolio_NM.xlsx
+++ b/2025_Course_Tracker_Portfolio_NM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\OneDrive\Documents2\GitHub\Cybersecurity Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F8579B-5E0B-4A3B-A2A8-B187F79F1E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3F7A95-284C-4305-8740-FF450627F10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD01DA7-E534-420E-81B3-A2A4503DB18F}"/>
   </bookViews>
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N5" sqref="N5"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>

</xml_diff>